<commit_message>
pdf invoice: fixed incorrect dates in generative case. Fixed local invoice page sizing. gradle: renamed task installToUserDirectory to installToUserHomeDir.
</commit_message>
<xml_diff>
--- a/src/main/resources/invoice_foreign.xlsx
+++ b/src/main/resources/invoice_foreign.xlsx
@@ -22,19 +22,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
-    <t xml:space="preserve">Baldin Sergey Invoice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Invoice date: October 26, 2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contract: dated as of September 9, 2016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Invoice number: 2018-10-SB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date of service: October 2018</t>
+    <t xml:space="preserve">Ivanov Ivan Invoice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invoice date: October 1, 2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contract: dated as of September 1, 2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invoice number: 2000-10-II</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date of service: October 2000</t>
   </si>
   <si>
     <t xml:space="preserve">Service Provided: Platform Development</t>
@@ -82,7 +82,7 @@
     <t xml:space="preserve">Bank Address and contact tel #</t>
   </si>
   <si>
-    <t xml:space="preserve">27 Kalanchevskaya str., Moscow, 107078, tel +7 495 755-58-58, SWIFT ALFARUMM</t>
+    <t xml:space="preserve">1 Lenina str., Moscow, 1000000, tel +7 495 755-58-58, SWIFT </t>
   </si>
   <si>
     <t xml:space="preserve">Beneficiary Name</t>
@@ -94,7 +94,23 @@
     <t xml:space="preserve">Your Address that you linked to that bank account</t>
   </si>
   <si>
-    <t xml:space="preserve">PR. LENINA, D. 1, KV. 1, MOSCOW, RUSSIA, 650000</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">PR. LENINA, D. 1, KV. 1, MOSCOW, RUSSIA, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">1000000</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -106,7 +122,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="[$$-409]\ #,##0"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -153,6 +169,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -390,7 +411,7 @@
   <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
pdf invoice: fixed incorrect dates in generative case. Fixed local invoice page sizing. (#2)
gradle: renamed task installToUserDirectory to installToUserHomeDir.
</commit_message>
<xml_diff>
--- a/src/main/resources/invoice_foreign.xlsx
+++ b/src/main/resources/invoice_foreign.xlsx
@@ -22,19 +22,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
-    <t xml:space="preserve">Baldin Sergey Invoice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Invoice date: October 26, 2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contract: dated as of September 9, 2016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Invoice number: 2018-10-SB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date of service: October 2018</t>
+    <t xml:space="preserve">Ivanov Ivan Invoice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invoice date: October 1, 2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contract: dated as of September 1, 2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invoice number: 2000-10-II</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date of service: October 2000</t>
   </si>
   <si>
     <t xml:space="preserve">Service Provided: Platform Development</t>
@@ -82,7 +82,7 @@
     <t xml:space="preserve">Bank Address and contact tel #</t>
   </si>
   <si>
-    <t xml:space="preserve">27 Kalanchevskaya str., Moscow, 107078, tel +7 495 755-58-58, SWIFT ALFARUMM</t>
+    <t xml:space="preserve">1 Lenina str., Moscow, 1000000, tel +7 495 755-58-58, SWIFT </t>
   </si>
   <si>
     <t xml:space="preserve">Beneficiary Name</t>
@@ -94,7 +94,23 @@
     <t xml:space="preserve">Your Address that you linked to that bank account</t>
   </si>
   <si>
-    <t xml:space="preserve">PR. LENINA, D. 1, KV. 1, MOSCOW, RUSSIA, 650000</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">PR. LENINA, D. 1, KV. 1, MOSCOW, RUSSIA, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">1000000</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -106,7 +122,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="[$$-409]\ #,##0"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -153,6 +169,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -390,7 +411,7 @@
   <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
OFFICE: fixed POI invoices.
</commit_message>
<xml_diff>
--- a/src/main/resources/invoice_foreign.xlsx
+++ b/src/main/resources/invoice_foreign.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t xml:space="preserve">Ivanov Ivan Invoice</t>
   </si>
@@ -64,53 +64,19 @@
     <t xml:space="preserve">Bank Name</t>
   </si>
   <si>
-    <t xml:space="preserve">AO «BANK»</t>
-  </si>
-  <si>
     <t xml:space="preserve">Account Number</t>
   </si>
   <si>
-    <t xml:space="preserve">0000000000000000000</t>
-  </si>
-  <si>
     <t xml:space="preserve">Bank Country</t>
   </si>
   <si>
-    <t xml:space="preserve">Russia</t>
-  </si>
-  <si>
     <t xml:space="preserve">Bank Address and contact tel #</t>
   </si>
   <si>
-    <t xml:space="preserve">1 Lenina str., Moscow, 1000000, tel +7 495 755-58-58, SWIFT </t>
-  </si>
-  <si>
     <t xml:space="preserve">Beneficiary Name</t>
   </si>
   <si>
-    <t xml:space="preserve">IP Ivanov Ivan Ivanovich</t>
-  </si>
-  <si>
     <t xml:space="preserve">Your Address that you linked to that bank account</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">PR. LENINA, D. 1, KV. 1, MOSCOW, RUSSIA, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">1000000</t>
-    </r>
   </si>
 </sst>
 </file>
@@ -122,7 +88,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="[$$-409]\ #,##0"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -169,11 +135,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -294,7 +255,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -381,6 +342,10 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
@@ -411,7 +376,7 @@
   <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -669,9 +634,7 @@
       <c r="A18" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="18" t="s">
-        <v>14</v>
-      </c>
+      <c r="B18" s="18"/>
       <c r="C18" s="18"/>
       <c r="D18" s="18"/>
       <c r="E18" s="18"/>
@@ -683,11 +646,9 @@
     </row>
     <row r="19" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="18" t="s">
-        <v>16</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="B19" s="18"/>
       <c r="C19" s="18"/>
       <c r="D19" s="18"/>
       <c r="E19" s="18"/>
@@ -699,11 +660,9 @@
     </row>
     <row r="20" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" s="18" t="s">
-        <v>18</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="B20" s="18"/>
       <c r="C20" s="18"/>
       <c r="D20" s="18"/>
       <c r="E20" s="18"/>
@@ -715,11 +674,9 @@
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="20" t="s">
-        <v>20</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="B21" s="20"/>
       <c r="C21" s="20"/>
       <c r="D21" s="20"/>
       <c r="E21" s="20"/>
@@ -803,14 +760,12 @@
     </row>
     <row r="28" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B28" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="22"/>
+        <v>17</v>
+      </c>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="23"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
@@ -819,11 +774,9 @@
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="B29" s="20" t="s">
-        <v>24</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="B29" s="20"/>
       <c r="C29" s="20"/>
       <c r="D29" s="20"/>
       <c r="E29" s="20"/>
@@ -906,11 +859,11 @@
       <c r="J35" s="2"/>
     </row>
     <row r="36" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="23"/>
-      <c r="B36" s="23"/>
-      <c r="C36" s="23"/>
-      <c r="D36" s="23"/>
-      <c r="E36" s="23"/>
+      <c r="A36" s="24"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="24"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="24"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
@@ -1038,10 +991,10 @@
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="B20:E20"/>
     <mergeCell ref="A21:A27"/>
-    <mergeCell ref="B21:E27"/>
+    <mergeCell ref="B21:D27"/>
     <mergeCell ref="B28:D28"/>
     <mergeCell ref="A29:A35"/>
-    <mergeCell ref="B29:E35"/>
+    <mergeCell ref="B29:D35"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.3"/>

</xml_diff>

<commit_message>
Feature/localized local bank model (#4)
* PDF, OFFICE, CONFIGS: Added LocalizedLocalBankingModel to work with local bank model in different invoices.

* OFFICE: fixed POI invoices.

* update readme
</commit_message>
<xml_diff>
--- a/src/main/resources/invoice_foreign.xlsx
+++ b/src/main/resources/invoice_foreign.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t xml:space="preserve">Ivanov Ivan Invoice</t>
   </si>
@@ -64,53 +64,19 @@
     <t xml:space="preserve">Bank Name</t>
   </si>
   <si>
-    <t xml:space="preserve">AO «BANK»</t>
-  </si>
-  <si>
     <t xml:space="preserve">Account Number</t>
   </si>
   <si>
-    <t xml:space="preserve">0000000000000000000</t>
-  </si>
-  <si>
     <t xml:space="preserve">Bank Country</t>
   </si>
   <si>
-    <t xml:space="preserve">Russia</t>
-  </si>
-  <si>
     <t xml:space="preserve">Bank Address and contact tel #</t>
   </si>
   <si>
-    <t xml:space="preserve">1 Lenina str., Moscow, 1000000, tel +7 495 755-58-58, SWIFT </t>
-  </si>
-  <si>
     <t xml:space="preserve">Beneficiary Name</t>
   </si>
   <si>
-    <t xml:space="preserve">IP Ivanov Ivan Ivanovich</t>
-  </si>
-  <si>
     <t xml:space="preserve">Your Address that you linked to that bank account</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">PR. LENINA, D. 1, KV. 1, MOSCOW, RUSSIA, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">1000000</t>
-    </r>
   </si>
 </sst>
 </file>
@@ -122,7 +88,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="[$$-409]\ #,##0"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -169,11 +135,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -294,7 +255,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -381,6 +342,10 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
@@ -411,7 +376,7 @@
   <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -669,9 +634,7 @@
       <c r="A18" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="18" t="s">
-        <v>14</v>
-      </c>
+      <c r="B18" s="18"/>
       <c r="C18" s="18"/>
       <c r="D18" s="18"/>
       <c r="E18" s="18"/>
@@ -683,11 +646,9 @@
     </row>
     <row r="19" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="18" t="s">
-        <v>16</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="B19" s="18"/>
       <c r="C19" s="18"/>
       <c r="D19" s="18"/>
       <c r="E19" s="18"/>
@@ -699,11 +660,9 @@
     </row>
     <row r="20" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" s="18" t="s">
-        <v>18</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="B20" s="18"/>
       <c r="C20" s="18"/>
       <c r="D20" s="18"/>
       <c r="E20" s="18"/>
@@ -715,11 +674,9 @@
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="20" t="s">
-        <v>20</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="B21" s="20"/>
       <c r="C21" s="20"/>
       <c r="D21" s="20"/>
       <c r="E21" s="20"/>
@@ -803,14 +760,12 @@
     </row>
     <row r="28" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B28" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="22"/>
+        <v>17</v>
+      </c>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="23"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
@@ -819,11 +774,9 @@
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="B29" s="20" t="s">
-        <v>24</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="B29" s="20"/>
       <c r="C29" s="20"/>
       <c r="D29" s="20"/>
       <c r="E29" s="20"/>
@@ -906,11 +859,11 @@
       <c r="J35" s="2"/>
     </row>
     <row r="36" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="23"/>
-      <c r="B36" s="23"/>
-      <c r="C36" s="23"/>
-      <c r="D36" s="23"/>
-      <c r="E36" s="23"/>
+      <c r="A36" s="24"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="24"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="24"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
@@ -1038,10 +991,10 @@
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="B20:E20"/>
     <mergeCell ref="A21:A27"/>
-    <mergeCell ref="B21:E27"/>
+    <mergeCell ref="B21:D27"/>
     <mergeCell ref="B28:D28"/>
     <mergeCell ref="A29:A35"/>
-    <mergeCell ref="B29:E35"/>
+    <mergeCell ref="B29:D35"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed klinter warnings. Fixed minor issues #TEST
</commit_message>
<xml_diff>
--- a/src/main/resources/invoice_foreign.xlsx
+++ b/src/main/resources/invoice_foreign.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fesswood/work/education/employeeInvoice/src/main/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fesswood/work/education/employeeInvoice/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC2EC4F-8434-6948-8514-892575BFD5BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{150C84F3-94F7-B84A-81A5-595453266CF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="460" windowWidth="20140" windowHeight="16500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="940" yWindow="460" windowWidth="20600" windowHeight="18760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -678,7 +678,7 @@
   <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -851,7 +851,7 @@
       <c r="A12" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="14">
+      <c r="B12" s="15">
         <v>0</v>
       </c>
       <c r="C12" s="12"/>

</xml_diff>